<commit_message>
Reconceptualización arbol decision (quito dos ramas de Asignar Ud Pob
</commit_message>
<xml_diff>
--- a/resumen_resultados.xlsx
+++ b/resumen_resultados.xlsx
@@ -147,7 +147,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8572500" cy="5715000"/>
+    <ext cx="8572500" cy="4762500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -511,40 +511,40 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Asignada Unidad Poblacional</t>
+          <t>Asignar Vía Nueva</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1188</v>
+        <v>1585</v>
       </c>
       <c r="C4" t="n">
-        <v>8.069007675066223</v>
+        <v>10.76546899409088</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Asignar Vía Nueva</t>
+          <t>Aislada</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>430</v>
+        <v>77</v>
       </c>
       <c r="C5" t="n">
-        <v>2.920600421109828</v>
+        <v>0.5229912381987367</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Aislada</t>
+          <t>Asignada Unidad Poblacional</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5229912381987367</v>
+        <v>0.2241391020851728</v>
       </c>
     </row>
   </sheetData>
@@ -629,12 +629,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>30 (2.7%)</t>
+          <t>0 (0.0%)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>29 (2.6%)</t>
+          <t>59 (5.4%)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -667,12 +667,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>128 (9.0%)</t>
+          <t>0 (0.0%)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>79 (5.6%)</t>
+          <t>207 (14.6%)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -705,12 +705,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>106 (15.2%)</t>
+          <t>1 (0.1%)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>56 (8.0%)</t>
+          <t>161 (23.1%)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -743,12 +743,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>591 (18.4%)</t>
+          <t>24 (0.7%)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>13 (0.4%)</t>
+          <t>580 (18.0%)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -781,12 +781,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>49 (5.1%)</t>
+          <t>3 (0.3%)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2 (0.2%)</t>
+          <t>48 (5.0%)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -819,12 +819,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>42 (26.9%)</t>
+          <t>0 (0.0%)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>28 (17.9%)</t>
+          <t>70 (44.9%)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -857,12 +857,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>88 (9.2%)</t>
+          <t>0 (0.0%)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>76 (8.0%)</t>
+          <t>164 (17.2%)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -895,12 +895,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>28 (4.2%)</t>
+          <t>1 (0.1%)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>15 (2.2%)</t>
+          <t>42 (6.2%)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -933,12 +933,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>24 (8.5%)</t>
+          <t>0 (0.0%)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>17 (6.0%)</t>
+          <t>41 (14.5%)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -971,12 +971,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>13 (3.4%)</t>
+          <t>2 (0.5%)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>4 (1.0%)</t>
+          <t>15 (3.9%)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1009,12 +1009,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3 (0.3%)</t>
+          <t>0 (0.0%)</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>4 (0.4%)</t>
+          <t>7 (0.7%)</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1047,12 +1047,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>15 (2.2%)</t>
+          <t>0 (0.0%)</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>53 (7.9%)</t>
+          <t>68 (10.2%)</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1085,12 +1085,12 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>14 (2.4%)</t>
+          <t>0 (0.0%)</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>14 (2.4%)</t>
+          <t>28 (4.9%)</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1123,12 +1123,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>3 (0.6%)</t>
+          <t>0 (0.0%)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>9 (1.7%)</t>
+          <t>12 (2.3%)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1161,12 +1161,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>9 (0.8%)</t>
+          <t>1 (0.1%)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2 (0.2%)</t>
+          <t>10 (0.9%)</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1199,12 +1199,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>23 (3.1%)</t>
+          <t>1 (0.1%)</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>4 (0.5%)</t>
+          <t>26 (3.5%)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1237,12 +1237,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>22 (8.1%)</t>
+          <t>0 (0.0%)</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>25 (9.2%)</t>
+          <t>47 (17.3%)</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1272,12 +1272,12 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1188 (8.1%)</t>
+          <t>33 (0.2%)</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>430 (2.9%)</t>
+          <t>1585 (10.8%)</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">

</xml_diff>